<commit_message>
Added micro SD card support
</commit_message>
<xml_diff>
--- a/Controller pin-toewijzingen.xlsx
+++ b/Controller pin-toewijzingen.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Toewijzingen" sheetId="2" r:id="rId1"/>
     <sheet name="Info" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="61">
   <si>
     <t>TTGO</t>
   </si>
@@ -183,6 +184,21 @@
   </si>
   <si>
     <t>Nog toewijzen</t>
+  </si>
+  <si>
+    <t>SD card</t>
+  </si>
+  <si>
+    <t>SCLK</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>CS</t>
   </si>
 </sst>
 </file>
@@ -282,7 +298,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -304,9 +320,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,6 +335,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -617,7 +634,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -671,10 +688,10 @@
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -688,10 +705,10 @@
       <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>36</v>
       </c>
     </row>
@@ -699,10 +716,10 @@
       <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>21</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>37</v>
       </c>
     </row>
@@ -710,18 +727,18 @@
       <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>22</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>17</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>39</v>
       </c>
     </row>
@@ -732,10 +749,10 @@
       <c r="B7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>2</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>32</v>
       </c>
     </row>
@@ -746,18 +763,18 @@
       <c r="B8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>15</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>13</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>25</v>
       </c>
     </row>
@@ -768,10 +785,10 @@
       <c r="B10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>12</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>26</v>
       </c>
     </row>
@@ -782,10 +799,10 @@
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>27</v>
       </c>
     </row>
@@ -796,10 +813,10 @@
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -813,10 +830,10 @@
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="7" t="s">
@@ -832,30 +849,62 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="14"/>
+      <c r="B21" s="13"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -870,7 +919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -885,7 +934,7 @@
     <col min="7" max="7" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="49.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -924,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="14" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="4" t="s">
@@ -956,7 +1005,7 @@
       <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="14">
         <v>0</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -985,7 +1034,7 @@
       <c r="G4" s="3">
         <v>36</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="14">
         <v>1</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -1014,7 +1063,7 @@
       <c r="G5" s="3">
         <v>37</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="14">
         <v>2</v>
       </c>
       <c r="K5" s="5" t="s">
@@ -1043,7 +1092,7 @@
       <c r="G6" s="3">
         <v>38</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="14">
         <v>3</v>
       </c>
       <c r="K6" s="5" t="s">
@@ -1069,7 +1118,7 @@
       <c r="G7" s="3">
         <v>39</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="14">
         <v>4</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -1093,7 +1142,7 @@
       <c r="G8" s="3">
         <v>32</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="14">
         <v>5</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1119,7 +1168,7 @@
       <c r="G9" s="3">
         <v>33</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="14">
         <v>6</v>
       </c>
       <c r="K9" s="5" t="s">
@@ -1145,7 +1194,7 @@
       <c r="G10" s="3">
         <v>25</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="14">
         <v>7</v>
       </c>
       <c r="K10" s="5" t="s">
@@ -1171,7 +1220,7 @@
       <c r="G11" s="3">
         <v>26</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="14">
         <v>8</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -1200,7 +1249,7 @@
       <c r="G12" s="3">
         <v>27</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="14">
         <v>9</v>
       </c>
       <c r="K12" s="5" t="s">
@@ -1232,7 +1281,7 @@
       <c r="H13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="14">
         <v>10</v>
       </c>
       <c r="K13" s="5" t="s">
@@ -1264,7 +1313,7 @@
       <c r="H14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="14">
         <v>11</v>
       </c>
       <c r="K14" s="5" t="s">
@@ -1281,7 +1330,7 @@
       <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="14">
         <v>12</v>
       </c>
       <c r="K15" s="5" t="s">
@@ -1295,7 +1344,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="J16" s="4">
+      <c r="J16" s="14">
         <v>13</v>
       </c>
       <c r="K16" s="5" t="s">
@@ -1307,7 +1356,7 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="10:13">
-      <c r="J17" s="4">
+      <c r="J17" s="14">
         <v>14</v>
       </c>
       <c r="K17" s="5" t="s">
@@ -1321,7 +1370,7 @@
       </c>
     </row>
     <row r="18" spans="10:13">
-      <c r="J18" s="4">
+      <c r="J18" s="14">
         <v>15</v>
       </c>
       <c r="K18" s="5" t="s">
@@ -1335,7 +1384,7 @@
       </c>
     </row>
     <row r="19" spans="10:13">
-      <c r="J19" s="4">
+      <c r="J19" s="14">
         <v>16</v>
       </c>
       <c r="K19" s="5" t="s">
@@ -1347,7 +1396,7 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="10:13">
-      <c r="J20" s="4">
+      <c r="J20" s="14">
         <v>17</v>
       </c>
       <c r="K20" s="5" t="s">
@@ -1359,7 +1408,7 @@
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="10:13">
-      <c r="J21" s="4">
+      <c r="J21" s="14">
         <v>18</v>
       </c>
       <c r="K21" s="5" t="s">
@@ -1371,7 +1420,7 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="10:13">
-      <c r="J22" s="4">
+      <c r="J22" s="14">
         <v>19</v>
       </c>
       <c r="K22" s="5" t="s">
@@ -1383,7 +1432,7 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="10:13">
-      <c r="J23" s="4">
+      <c r="J23" s="14">
         <v>21</v>
       </c>
       <c r="K23" s="5" t="s">
@@ -1395,7 +1444,7 @@
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="10:13">
-      <c r="J24" s="9">
+      <c r="J24" s="14">
         <v>22</v>
       </c>
       <c r="K24" s="5" t="s">
@@ -1407,7 +1456,7 @@
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="10:13">
-      <c r="J25" s="4">
+      <c r="J25" s="14">
         <v>23</v>
       </c>
       <c r="K25" s="5" t="s">
@@ -1419,7 +1468,7 @@
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="10:13">
-      <c r="J26" s="9">
+      <c r="J26" s="14">
         <v>25</v>
       </c>
       <c r="K26" s="5" t="s">
@@ -1431,7 +1480,7 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="10:13">
-      <c r="J27" s="9">
+      <c r="J27" s="14">
         <v>26</v>
       </c>
       <c r="K27" s="5" t="s">
@@ -1443,7 +1492,7 @@
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="10:13">
-      <c r="J28" s="4">
+      <c r="J28" s="14">
         <v>27</v>
       </c>
       <c r="K28" s="5" t="s">
@@ -1455,7 +1504,7 @@
       <c r="M28" s="5"/>
     </row>
     <row r="29" spans="10:13">
-      <c r="J29" s="4">
+      <c r="J29" s="14">
         <v>32</v>
       </c>
       <c r="K29" s="5" t="s">
@@ -1467,7 +1516,7 @@
       <c r="M29" s="5"/>
     </row>
     <row r="30" spans="10:13">
-      <c r="J30" s="4">
+      <c r="J30" s="14">
         <v>33</v>
       </c>
       <c r="K30" s="5" t="s">
@@ -1479,7 +1528,7 @@
       <c r="M30" s="5"/>
     </row>
     <row r="31" spans="10:13">
-      <c r="J31" s="4">
+      <c r="J31" s="14">
         <v>34</v>
       </c>
       <c r="K31" s="5" t="s">
@@ -1491,7 +1540,7 @@
       </c>
     </row>
     <row r="32" spans="10:13">
-      <c r="J32" s="4">
+      <c r="J32" s="14">
         <v>35</v>
       </c>
       <c r="K32" s="5" t="s">
@@ -1503,7 +1552,7 @@
       </c>
     </row>
     <row r="33" spans="10:13">
-      <c r="J33" s="4">
+      <c r="J33" s="14">
         <v>36</v>
       </c>
       <c r="K33" s="5" t="s">
@@ -1515,7 +1564,7 @@
       </c>
     </row>
     <row r="34" spans="10:13">
-      <c r="J34" s="4">
+      <c r="J34" s="14">
         <v>39</v>
       </c>
       <c r="K34" s="5" t="s">
@@ -1540,4 +1589,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update software en pin-toewijzingen
</commit_message>
<xml_diff>
--- a/Controller pin-toewijzingen.xlsx
+++ b/Controller pin-toewijzingen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="68">
   <si>
     <t>TTGO</t>
   </si>
@@ -156,9 +156,6 @@
     <t>BCLK</t>
   </si>
   <si>
-    <t>DATA</t>
-  </si>
-  <si>
     <t>LRCLK</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>Voeding</t>
   </si>
   <si>
-    <t>Onbekend</t>
-  </si>
-  <si>
     <t>Nog toewijzen</t>
   </si>
   <si>
@@ -199,6 +193,33 @@
   </si>
   <si>
     <t>CS</t>
+  </si>
+  <si>
+    <t>RFID</t>
+  </si>
+  <si>
+    <t>LED rings</t>
+  </si>
+  <si>
+    <t>LED display</t>
+  </si>
+  <si>
+    <t>Touch</t>
+  </si>
+  <si>
+    <t>CLK</t>
+  </si>
+  <si>
+    <t>SH/LDn</t>
+  </si>
+  <si>
+    <t>Menutoets</t>
+  </si>
+  <si>
+    <t>DOUT</t>
+  </si>
+  <si>
+    <t>DIN</t>
   </si>
 </sst>
 </file>
@@ -250,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,12 +293,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,9 +326,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,9 +341,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,6 +348,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -634,281 +649,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="7" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="9">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9">
+        <v>22</v>
+      </c>
+      <c r="F5" s="10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="D6" s="9">
+        <v>17</v>
+      </c>
+      <c r="F6" s="10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="10">
+        <v>15</v>
+      </c>
+      <c r="F8" s="9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="D9" s="9">
+        <v>13</v>
+      </c>
+      <c r="F9" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="10">
+        <v>12</v>
+      </c>
+      <c r="F10" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="D16" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="D17" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="D18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="11">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="10">
-        <v>21</v>
-      </c>
-      <c r="F4" s="11">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="10">
-        <v>22</v>
-      </c>
-      <c r="F5" s="11">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="D6" s="10">
-        <v>17</v>
-      </c>
-      <c r="F6" s="11">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="11">
-        <v>2</v>
-      </c>
-      <c r="F7" s="10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="11">
-        <v>15</v>
-      </c>
-      <c r="F8" s="10">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="D9" s="10">
-        <v>13</v>
-      </c>
-      <c r="F9" s="10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="11">
-        <v>12</v>
-      </c>
-      <c r="F10" s="10">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="10">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="E14" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="D16" s="9" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="D17" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="D18" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="D19" s="12" t="s">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="13" t="s">
+      <c r="B21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="13"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="7" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="7" t="s">
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" s="11" t="s">
         <v>60</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -934,7 +1032,7 @@
     <col min="7" max="7" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="49.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -943,23 +1041,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="11.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -973,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="4" t="s">
@@ -1005,7 +1103,7 @@
       <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="12">
         <v>0</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -1034,7 +1132,7 @@
       <c r="G4" s="3">
         <v>36</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="12">
         <v>1</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -1063,7 +1161,7 @@
       <c r="G5" s="3">
         <v>37</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="12">
         <v>2</v>
       </c>
       <c r="K5" s="5" t="s">
@@ -1092,7 +1190,7 @@
       <c r="G6" s="3">
         <v>38</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="12">
         <v>3</v>
       </c>
       <c r="K6" s="5" t="s">
@@ -1118,7 +1216,7 @@
       <c r="G7" s="3">
         <v>39</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="12">
         <v>4</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -1142,7 +1240,7 @@
       <c r="G8" s="3">
         <v>32</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="12">
         <v>5</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1168,7 +1266,7 @@
       <c r="G9" s="3">
         <v>33</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="12">
         <v>6</v>
       </c>
       <c r="K9" s="5" t="s">
@@ -1194,7 +1292,7 @@
       <c r="G10" s="3">
         <v>25</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="12">
         <v>7</v>
       </c>
       <c r="K10" s="5" t="s">
@@ -1220,7 +1318,7 @@
       <c r="G11" s="3">
         <v>26</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="12">
         <v>8</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -1249,7 +1347,7 @@
       <c r="G12" s="3">
         <v>27</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="12">
         <v>9</v>
       </c>
       <c r="K12" s="5" t="s">
@@ -1281,7 +1379,7 @@
       <c r="H13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="12">
         <v>10</v>
       </c>
       <c r="K13" s="5" t="s">
@@ -1313,7 +1411,7 @@
       <c r="H14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="12">
         <v>11</v>
       </c>
       <c r="K14" s="5" t="s">
@@ -1330,7 +1428,7 @@
       <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="12">
         <v>12</v>
       </c>
       <c r="K15" s="5" t="s">
@@ -1344,7 +1442,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="J16" s="14">
+      <c r="J16" s="12">
         <v>13</v>
       </c>
       <c r="K16" s="5" t="s">
@@ -1356,7 +1454,7 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="10:13">
-      <c r="J17" s="14">
+      <c r="J17" s="12">
         <v>14</v>
       </c>
       <c r="K17" s="5" t="s">
@@ -1370,7 +1468,7 @@
       </c>
     </row>
     <row r="18" spans="10:13">
-      <c r="J18" s="14">
+      <c r="J18" s="12">
         <v>15</v>
       </c>
       <c r="K18" s="5" t="s">
@@ -1384,7 +1482,7 @@
       </c>
     </row>
     <row r="19" spans="10:13">
-      <c r="J19" s="14">
+      <c r="J19" s="12">
         <v>16</v>
       </c>
       <c r="K19" s="5" t="s">
@@ -1396,7 +1494,7 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="10:13">
-      <c r="J20" s="14">
+      <c r="J20" s="12">
         <v>17</v>
       </c>
       <c r="K20" s="5" t="s">
@@ -1408,7 +1506,7 @@
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="10:13">
-      <c r="J21" s="14">
+      <c r="J21" s="12">
         <v>18</v>
       </c>
       <c r="K21" s="5" t="s">
@@ -1420,7 +1518,7 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="10:13">
-      <c r="J22" s="14">
+      <c r="J22" s="12">
         <v>19</v>
       </c>
       <c r="K22" s="5" t="s">
@@ -1432,7 +1530,7 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="10:13">
-      <c r="J23" s="14">
+      <c r="J23" s="12">
         <v>21</v>
       </c>
       <c r="K23" s="5" t="s">
@@ -1444,7 +1542,7 @@
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="10:13">
-      <c r="J24" s="14">
+      <c r="J24" s="12">
         <v>22</v>
       </c>
       <c r="K24" s="5" t="s">
@@ -1456,7 +1554,7 @@
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="10:13">
-      <c r="J25" s="14">
+      <c r="J25" s="12">
         <v>23</v>
       </c>
       <c r="K25" s="5" t="s">
@@ -1468,7 +1566,7 @@
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="10:13">
-      <c r="J26" s="14">
+      <c r="J26" s="12">
         <v>25</v>
       </c>
       <c r="K26" s="5" t="s">
@@ -1480,7 +1578,7 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="10:13">
-      <c r="J27" s="14">
+      <c r="J27" s="12">
         <v>26</v>
       </c>
       <c r="K27" s="5" t="s">
@@ -1492,7 +1590,7 @@
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="10:13">
-      <c r="J28" s="14">
+      <c r="J28" s="12">
         <v>27</v>
       </c>
       <c r="K28" s="5" t="s">
@@ -1504,7 +1602,7 @@
       <c r="M28" s="5"/>
     </row>
     <row r="29" spans="10:13">
-      <c r="J29" s="14">
+      <c r="J29" s="12">
         <v>32</v>
       </c>
       <c r="K29" s="5" t="s">
@@ -1516,7 +1614,7 @@
       <c r="M29" s="5"/>
     </row>
     <row r="30" spans="10:13">
-      <c r="J30" s="14">
+      <c r="J30" s="12">
         <v>33</v>
       </c>
       <c r="K30" s="5" t="s">
@@ -1528,7 +1626,7 @@
       <c r="M30" s="5"/>
     </row>
     <row r="31" spans="10:13">
-      <c r="J31" s="14">
+      <c r="J31" s="12">
         <v>34</v>
       </c>
       <c r="K31" s="5" t="s">
@@ -1540,7 +1638,7 @@
       </c>
     </row>
     <row r="32" spans="10:13">
-      <c r="J32" s="14">
+      <c r="J32" s="12">
         <v>35</v>
       </c>
       <c r="K32" s="5" t="s">
@@ -1552,7 +1650,7 @@
       </c>
     </row>
     <row r="33" spans="10:13">
-      <c r="J33" s="14">
+      <c r="J33" s="12">
         <v>36</v>
       </c>
       <c r="K33" s="5" t="s">
@@ -1564,7 +1662,7 @@
       </c>
     </row>
     <row r="34" spans="10:13">
-      <c r="J34" s="14">
+      <c r="J34" s="12">
         <v>39</v>
       </c>
       <c r="K34" s="5" t="s">

</xml_diff>